<commit_message>
Removed excel file. Refactoring.
</commit_message>
<xml_diff>
--- a/res/thermo.xlsx
+++ b/res/thermo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nichollsh/Projects/THEMIS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11FCCB3B-9AED-4445-831A-90E787DCE203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E542BC-22A4-954B-81FD-F6759694D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{331180BC-B4C8-F347-AEB5-8872F2FBBC91}"/>
   </bookViews>
@@ -591,14 +591,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FB1A5-96FD-6C4B-A9FD-DD03FA6F5C64}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -631,7 +632,6 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
@@ -651,7 +651,6 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
@@ -671,7 +670,6 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
@@ -691,7 +689,6 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
@@ -711,7 +708,6 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
@@ -731,7 +727,6 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
@@ -751,7 +746,6 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
@@ -771,7 +765,6 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
@@ -791,7 +784,6 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
@@ -811,7 +803,6 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
@@ -831,7 +822,6 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
@@ -851,7 +841,6 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
@@ -871,7 +860,6 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
@@ -891,7 +879,6 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
@@ -911,7 +898,6 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
@@ -931,7 +917,6 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
@@ -951,7 +936,6 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
@@ -971,7 +955,6 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
@@ -991,7 +974,6 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
@@ -1011,7 +993,6 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
@@ -1031,7 +1012,6 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
@@ -1051,7 +1031,6 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
@@ -1071,7 +1050,6 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
@@ -1091,7 +1069,6 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
@@ -1111,7 +1088,6 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
@@ -1131,7 +1107,6 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
@@ -1151,7 +1126,6 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
@@ -1171,7 +1145,6 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
@@ -1191,7 +1164,6 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
@@ -1211,7 +1183,6 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
@@ -1231,7 +1202,6 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
@@ -1251,7 +1221,6 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
@@ -1271,7 +1240,6 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
@@ -1291,7 +1259,6 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
@@ -1311,7 +1278,6 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
@@ -1331,7 +1297,6 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
@@ -1351,7 +1316,6 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
@@ -1371,7 +1335,6 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
@@ -1391,7 +1354,6 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
@@ -1411,7 +1373,6 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
@@ -1431,7 +1392,6 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
@@ -1451,7 +1411,6 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
@@ -1471,7 +1430,6 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
@@ -1491,7 +1449,6 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
@@ -1511,7 +1468,6 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
@@ -1531,7 +1487,6 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
@@ -1551,7 +1506,6 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
@@ -1571,7 +1525,6 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
@@ -1591,7 +1544,6 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
@@ -1611,7 +1563,6 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
@@ -1631,7 +1582,6 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
@@ -1651,7 +1601,6 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
@@ -1671,7 +1620,6 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
@@ -1691,7 +1639,6 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
@@ -1711,7 +1658,6 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
@@ -1722,16 +1668,16 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:N62">
+  <conditionalFormatting sqref="B2:G62 I2:N62">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>0.0000000000000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added prescribed h2o moist adiabat. Doesn't recover greenhouse limit
</commit_message>
<xml_diff>
--- a/res/thermo.xlsx
+++ b/res/thermo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nichollsh/Projects/THEMIS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E542BC-22A4-954B-81FD-F6759694D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A684CE9B-C231-3A4F-8186-F0491527917C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{331180BC-B4C8-F347-AEB5-8872F2FBBC91}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>H2O</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>Lvap (J/kg)</t>
+  </si>
+  <si>
+    <t>Ttrip (K)</t>
+  </si>
+  <si>
+    <t>Ptrip (Pa)</t>
   </si>
 </sst>
 </file>
@@ -220,7 +226,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -253,7 +259,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,20 +595,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FB1A5-96FD-6C4B-A9FD-DD03FA6F5C64}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -615,8 +621,14 @@
       <c r="D1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -629,13 +641,17 @@
       <c r="D2" s="1">
         <v>2493000</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="F2" s="1">
+        <v>611</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -648,13 +664,17 @@
       <c r="D3" s="1">
         <v>397000</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1">
+        <v>216.54</v>
+      </c>
+      <c r="F3" s="1">
+        <v>518500</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -667,13 +687,17 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -686,13 +710,17 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -705,13 +733,17 @@
       <c r="D6" s="1">
         <v>214285.7</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>67.95</v>
+      </c>
+      <c r="F6" s="1">
+        <v>15300</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -724,13 +756,17 @@
       <c r="D7" s="1">
         <v>536000</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1">
+        <v>90.67</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11700</v>
+      </c>
       <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -743,13 +779,17 @@
       <c r="D8" s="1">
         <v>242000</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1">
+        <v>54.3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>150</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -762,13 +802,17 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -781,13 +825,17 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
       <c r="G10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -800,13 +848,17 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -819,13 +871,17 @@
       <c r="D12" s="1">
         <v>1658000</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1">
+        <v>195.4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6100</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -838,13 +894,17 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
       <c r="G13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -857,13 +917,17 @@
       <c r="D14" s="1">
         <v>218000</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>63.14</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12530</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -876,13 +940,17 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
       <c r="G15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -895,13 +963,17 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
       <c r="G16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -914,13 +986,17 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -933,13 +1009,17 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
       <c r="G18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -952,13 +1032,17 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
       <c r="G19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -971,13 +1055,17 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
       <c r="G20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -990,13 +1078,17 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
       <c r="G21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1009,13 +1101,17 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
       <c r="G22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1028,13 +1124,17 @@
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
       <c r="G23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1047,13 +1147,17 @@
       <c r="D24" s="1">
         <v>454000</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="1">
+        <v>13.95</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7200</v>
+      </c>
       <c r="G24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1066,13 +1170,17 @@
       <c r="D25" s="1">
         <v>20300</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="1">
+        <v>2.17</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5070</v>
+      </c>
       <c r="G25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1085,13 +1193,17 @@
       <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
       <c r="G26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1104,13 +1216,17 @@
       <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
       <c r="G27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1123,13 +1239,17 @@
       <c r="D28" s="1">
         <v>0</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
       <c r="G28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1142,13 +1262,17 @@
       <c r="D29" s="1">
         <v>0</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
       <c r="G29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1161,13 +1285,17 @@
       <c r="D30" s="1">
         <v>0</v>
       </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
       <c r="G30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1180,13 +1308,17 @@
       <c r="D31" s="1">
         <v>0</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
       <c r="G31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1199,13 +1331,17 @@
       <c r="D32" s="1">
         <v>0</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
       <c r="G32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1218,13 +1354,17 @@
       <c r="D33" s="1">
         <v>0</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
       <c r="G33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1237,13 +1377,17 @@
       <c r="D34" s="1">
         <v>0</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
       <c r="G34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1256,13 +1400,17 @@
       <c r="D35" s="1">
         <v>0</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
       <c r="G35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1275,13 +1423,17 @@
       <c r="D36" s="1">
         <v>0</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
       <c r="G36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1294,13 +1446,17 @@
       <c r="D37" s="1">
         <v>0</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
       <c r="G37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1313,13 +1469,17 @@
       <c r="D38" s="1">
         <v>0</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
       <c r="G38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1332,13 +1492,17 @@
       <c r="D39" s="1">
         <v>0</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
       <c r="G39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1351,13 +1515,17 @@
       <c r="D40" s="1">
         <v>0</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
       <c r="G40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1370,13 +1538,17 @@
       <c r="D41" s="1">
         <v>0</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
       <c r="G41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1389,13 +1561,17 @@
       <c r="D42" s="1">
         <v>0</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
       <c r="G42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1408,13 +1584,17 @@
       <c r="D43" s="1">
         <v>0</v>
       </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
       <c r="G43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1427,13 +1607,17 @@
       <c r="D44" s="1">
         <v>0</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
       <c r="G44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1446,13 +1630,17 @@
       <c r="D45" s="1">
         <v>0</v>
       </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="E45" s="1">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
       <c r="G45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1465,13 +1653,17 @@
       <c r="D46" s="1">
         <v>0</v>
       </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
       <c r="G46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1484,13 +1676,17 @@
       <c r="D47" s="1">
         <v>0</v>
       </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
       <c r="G47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1503,13 +1699,17 @@
       <c r="D48" s="1">
         <v>0</v>
       </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
       <c r="G48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1522,13 +1722,17 @@
       <c r="D49" s="1">
         <v>0</v>
       </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="E49" s="1">
+        <v>0</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0</v>
+      </c>
       <c r="G49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1541,13 +1745,17 @@
       <c r="D50" s="1">
         <v>0</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
       <c r="G50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1560,13 +1768,17 @@
       <c r="D51" s="1">
         <v>0</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
       <c r="G51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1579,13 +1791,17 @@
       <c r="D52" s="1">
         <v>0</v>
       </c>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
       <c r="G52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1598,13 +1814,17 @@
       <c r="D53" s="1">
         <v>0</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
       <c r="G53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1617,13 +1837,17 @@
       <c r="D54" s="1">
         <v>0</v>
       </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
       <c r="G54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1636,13 +1860,17 @@
       <c r="D55" s="1">
         <v>0</v>
       </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
       <c r="G55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1655,24 +1883,33 @@
       <c r="D56" s="1">
         <v>0</v>
       </c>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
       <c r="G56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G62 I2:N62">
+  <conditionalFormatting sqref="B2:G62 L2:N62">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>0.0000000000000000001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K62">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
       <formula>0.0000000000000000001</formula>
     </cfRule>

</xml_diff>